<commit_message>
Add fix O&M costs for existing ICEs
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_TRA_Early_Retirement.xlsx
+++ b/SuppXLS/Scen_TRA_Early_Retirement.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\VEDA_Models\~g2v_Irish-TIMES-model\tra-updates\SuppXLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76FC3D99-1551-4A90-999A-F5CEF7E4B545}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79C627BF-5D5D-44F1-A2F8-6866BAAAB6F2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -160,7 +160,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="88">
   <si>
     <t>Pset_CI</t>
   </si>
@@ -438,6 +438,12 @@
   </si>
   <si>
     <t>N</t>
+  </si>
+  <si>
+    <t>T-CAR-ICE*</t>
+  </si>
+  <si>
+    <t>FIXOM</t>
   </si>
 </sst>
 </file>
@@ -1798,8 +1804,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AQ15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView tabSelected="1" topLeftCell="R1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AJ14" sqref="AJ14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2086,9 +2092,101 @@
         <v>0</v>
       </c>
       <c r="AJ4" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="AK4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="D5" t="s">
+        <v>87</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5" s="14">
+        <v>1</v>
+      </c>
+      <c r="J5" s="14">
+        <v>1</v>
+      </c>
+      <c r="K5" s="14">
+        <v>1</v>
+      </c>
+      <c r="L5" s="14">
+        <v>1</v>
+      </c>
+      <c r="M5" s="14">
+        <v>1</v>
+      </c>
+      <c r="N5" s="14">
+        <v>1</v>
+      </c>
+      <c r="O5" s="14">
+        <v>1</v>
+      </c>
+      <c r="P5" s="14">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="14">
+        <v>1</v>
+      </c>
+      <c r="R5" s="14">
+        <v>1</v>
+      </c>
+      <c r="S5" s="14">
+        <v>1</v>
+      </c>
+      <c r="T5" s="14">
+        <v>1</v>
+      </c>
+      <c r="U5" s="14">
+        <v>1</v>
+      </c>
+      <c r="V5" s="14">
+        <v>1</v>
+      </c>
+      <c r="W5" s="14">
+        <v>1</v>
+      </c>
+      <c r="X5" s="14">
+        <v>1</v>
+      </c>
+      <c r="Y5" s="14">
+        <v>1</v>
+      </c>
+      <c r="Z5" s="14">
+        <v>1</v>
+      </c>
+      <c r="AA5" s="14">
+        <v>1</v>
+      </c>
+      <c r="AB5" s="14">
+        <v>1</v>
+      </c>
+      <c r="AC5" s="14">
+        <v>1</v>
+      </c>
+      <c r="AD5" s="14">
+        <v>1</v>
+      </c>
+      <c r="AE5" s="14">
+        <v>1</v>
+      </c>
+      <c r="AF5" s="14">
+        <v>1</v>
+      </c>
+      <c r="AG5" s="14">
+        <v>1</v>
+      </c>
+      <c r="AH5" s="14">
+        <v>1</v>
+      </c>
+      <c r="AJ5" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="AK5" s="14" t="s">
         <v>81</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Modify early retirement table
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_TRA_Early_Retirement.xlsx
+++ b/SuppXLS/Scen_TRA_Early_Retirement.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79C627BF-5D5D-44F1-A2F8-6866BAAAB6F2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{880A3A54-FA8A-4637-AE83-4836E415F9A3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -160,7 +160,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="85">
   <si>
     <t>Pset_CI</t>
   </si>
@@ -422,16 +422,7 @@
     <t>other_indexes</t>
   </si>
   <si>
-    <t>T-CAR-BEV*</t>
-  </si>
-  <si>
     <t>*Existing*</t>
-  </si>
-  <si>
-    <t>INVCOST</t>
-  </si>
-  <si>
-    <t>*New</t>
   </si>
   <si>
     <t>RCAP_BND</t>
@@ -601,7 +592,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -626,9 +617,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1802,10 +1790,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AQ15"/>
+  <dimension ref="A1:AQ17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AJ14" sqref="AJ14"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11:K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2005,10 +1993,10 @@
     </row>
     <row r="4" spans="1:43" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D4" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="H4" s="14">
         <v>0</v>
@@ -2092,15 +2080,15 @@
         <v>0</v>
       </c>
       <c r="AJ4" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="AK4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:43" x14ac:dyDescent="0.3">
       <c r="D5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="H5">
         <v>1</v>
@@ -2184,67 +2172,88 @@
         <v>1</v>
       </c>
       <c r="AJ5" s="14" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="AK5" s="14" t="s">
-        <v>81</v>
-      </c>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="14"/>
+    </row>
+    <row r="12" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="14"/>
     </row>
     <row r="13" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="C13" s="1" t="s">
-        <v>16</v>
-      </c>
+      <c r="C13" s="14"/>
       <c r="D13" s="14"/>
       <c r="E13" s="14"/>
       <c r="F13" s="14"/>
       <c r="G13" s="14"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-    </row>
-    <row r="14" spans="1:43" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C14" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="G14" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="H14" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="I14" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="J14" s="6" t="s">
-        <v>11</v>
-      </c>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="14"/>
+    </row>
+    <row r="14" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="14"/>
     </row>
     <row r="15" spans="1:43" x14ac:dyDescent="0.3">
       <c r="C15" s="14"/>
       <c r="D15" s="14"/>
-      <c r="E15" s="14" t="s">
-        <v>82</v>
-      </c>
+      <c r="E15" s="14"/>
       <c r="F15" s="14"/>
-      <c r="G15" s="15">
-        <v>-5</v>
-      </c>
+      <c r="G15" s="14"/>
       <c r="H15" s="14"/>
-      <c r="I15" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="J15" s="14" t="s">
-        <v>83</v>
-      </c>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="14"/>
+    </row>
+    <row r="16" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="14"/>
+    </row>
+    <row r="17" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="14"/>
+      <c r="K17" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Move increased FOM for existing cars to a separate file
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_TRA_Early_Retirement.xlsx
+++ b/SuppXLS/Scen_TRA_Early_Retirement.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Irish-TIMES-model\SuppXLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{880A3A54-FA8A-4637-AE83-4836E415F9A3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1B0DD72-2C20-4355-ADA4-7EA41C065A25}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="15" r:id="rId1"/>
@@ -160,7 +160,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="84">
   <si>
     <t>Pset_CI</t>
   </si>
@@ -431,10 +431,7 @@
     <t>N</t>
   </si>
   <si>
-    <t>T-CAR-ICE*</t>
-  </si>
-  <si>
-    <t>FIXOM</t>
+    <t>T-CAR-*</t>
   </si>
 </sst>
 </file>
@@ -651,7 +648,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>22860</xdr:colOff>
+          <xdr:colOff>19050</xdr:colOff>
           <xdr:row>3</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -1029,40 +1026,40 @@
       <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.109375" style="7" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" style="7" customWidth="1"/>
-    <col min="3" max="3" width="3.109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.5546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.44140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.88671875" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.88671875" style="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.44140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="5.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.5546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.5546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.33203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="6.109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="5.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="5.5546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="5.88671875" style="7" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="6.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="4.88671875" style="7" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="7.5546875" style="7" customWidth="1"/>
-    <col min="25" max="25" width="6.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="6.109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" style="7" customWidth="1"/>
+    <col min="3" max="3" width="3.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="5.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="5.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="5.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="6.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="4.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="7.5703125" style="7" customWidth="1"/>
+    <col min="25" max="25" width="6.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="6.140625" style="7" bestFit="1" customWidth="1"/>
     <col min="27" max="28" width="6" style="7" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="5.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="6.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="31" max="16384" width="9.109375" style="7"/>
+    <col min="29" max="29" width="5.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="6.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="31" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="C3" s="8" t="str" cm="1">
         <f t="array" ref="C3">INDEX(C5:C7,$A$4)</f>
         <v>IE</v>
@@ -1176,12 +1173,12 @@
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>45</v>
       </c>
@@ -1296,7 +1293,7 @@
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>48</v>
       </c>
@@ -1413,7 +1410,7 @@
         <v>*IE-MN</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>49</v>
       </c>
@@ -1530,7 +1527,7 @@
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="10" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
         <v>50</v>
       </c>
@@ -1538,7 +1535,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>52</v>
       </c>
@@ -1546,7 +1543,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
         <v>53</v>
       </c>
@@ -1554,7 +1551,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
         <v>54</v>
       </c>
@@ -1562,7 +1559,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
         <v>55</v>
       </c>
@@ -1570,7 +1567,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
         <v>56</v>
       </c>
@@ -1578,7 +1575,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>57</v>
       </c>
@@ -1586,7 +1583,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>58</v>
       </c>
@@ -1594,7 +1591,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>59</v>
       </c>
@@ -1602,7 +1599,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>60</v>
       </c>
@@ -1610,7 +1607,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
         <v>61</v>
       </c>
@@ -1618,7 +1615,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>62</v>
       </c>
@@ -1626,7 +1623,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
         <v>63</v>
       </c>
@@ -1634,7 +1631,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
         <v>64</v>
       </c>
@@ -1642,7 +1639,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
         <v>65</v>
       </c>
@@ -1650,7 +1647,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
         <v>66</v>
       </c>
@@ -1658,7 +1655,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
         <v>67</v>
       </c>
@@ -1666,7 +1663,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
         <v>68</v>
       </c>
@@ -1674,7 +1671,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
         <v>69</v>
       </c>
@@ -1682,7 +1679,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
         <v>70</v>
       </c>
@@ -1690,7 +1687,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
         <v>71</v>
       </c>
@@ -1698,7 +1695,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
         <v>72</v>
       </c>
@@ -1706,7 +1703,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
         <v>73</v>
       </c>
@@ -1714,7 +1711,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="s">
         <v>74</v>
       </c>
@@ -1722,7 +1719,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
         <v>75</v>
       </c>
@@ -1730,7 +1727,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="s">
         <v>76</v>
       </c>
@@ -1738,7 +1735,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="12" t="s">
         <v>77</v>
       </c>
@@ -1746,7 +1743,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="13" t="s">
         <v>78</v>
       </c>
@@ -1772,7 +1769,7 @@
                   </from>
                   <to>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>22860</xdr:colOff>
+                    <xdr:colOff>19050</xdr:colOff>
                     <xdr:row>3</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </to>
@@ -1793,36 +1790,36 @@
   <dimension ref="A1:AQ17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11:K17"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="33" width="10.6640625" customWidth="1"/>
-    <col min="34" max="34" width="10.6640625" style="7" customWidth="1"/>
-    <col min="35" max="35" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="12.21875" style="14" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="33" width="10.7109375" customWidth="1"/>
+    <col min="34" max="34" width="10.7109375" style="7" customWidth="1"/>
+    <col min="35" max="35" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="12.28515625" style="14" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="8.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:43" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
@@ -1836,7 +1833,7 @@
       <c r="AP2" s="3"/>
       <c r="AQ2" s="3"/>
     </row>
-    <row r="3" spans="1:43" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="4" t="s">
         <v>9</v>
       </c>
@@ -1991,7 +1988,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:43" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>82</v>
       </c>
@@ -2086,99 +2083,37 @@
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="D5" t="s">
-        <v>84</v>
-      </c>
-      <c r="H5">
-        <v>1</v>
-      </c>
-      <c r="I5" s="14">
-        <v>1</v>
-      </c>
-      <c r="J5" s="14">
-        <v>1</v>
-      </c>
-      <c r="K5" s="14">
-        <v>1</v>
-      </c>
-      <c r="L5" s="14">
-        <v>1</v>
-      </c>
-      <c r="M5" s="14">
-        <v>1</v>
-      </c>
-      <c r="N5" s="14">
-        <v>1</v>
-      </c>
-      <c r="O5" s="14">
-        <v>1</v>
-      </c>
-      <c r="P5" s="14">
-        <v>1</v>
-      </c>
-      <c r="Q5" s="14">
-        <v>1</v>
-      </c>
-      <c r="R5" s="14">
-        <v>1</v>
-      </c>
-      <c r="S5" s="14">
-        <v>1</v>
-      </c>
-      <c r="T5" s="14">
-        <v>1</v>
-      </c>
-      <c r="U5" s="14">
-        <v>1</v>
-      </c>
-      <c r="V5" s="14">
-        <v>1</v>
-      </c>
-      <c r="W5" s="14">
-        <v>1</v>
-      </c>
-      <c r="X5" s="14">
-        <v>1</v>
-      </c>
-      <c r="Y5" s="14">
-        <v>1</v>
-      </c>
-      <c r="Z5" s="14">
-        <v>1</v>
-      </c>
-      <c r="AA5" s="14">
-        <v>1</v>
-      </c>
-      <c r="AB5" s="14">
-        <v>1</v>
-      </c>
-      <c r="AC5" s="14">
-        <v>1</v>
-      </c>
-      <c r="AD5" s="14">
-        <v>1</v>
-      </c>
-      <c r="AE5" s="14">
-        <v>1</v>
-      </c>
-      <c r="AF5" s="14">
-        <v>1</v>
-      </c>
-      <c r="AG5" s="14">
-        <v>1</v>
-      </c>
-      <c r="AH5" s="14">
-        <v>1</v>
-      </c>
-      <c r="AJ5" s="14" t="s">
-        <v>83</v>
-      </c>
-      <c r="AK5" s="14" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="11" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="14"/>
+      <c r="N5" s="14"/>
+      <c r="O5" s="14"/>
+      <c r="P5" s="14"/>
+      <c r="Q5" s="14"/>
+      <c r="R5" s="14"/>
+      <c r="S5" s="14"/>
+      <c r="T5" s="14"/>
+      <c r="U5" s="14"/>
+      <c r="V5" s="14"/>
+      <c r="W5" s="14"/>
+      <c r="X5" s="14"/>
+      <c r="Y5" s="14"/>
+      <c r="Z5" s="14"/>
+      <c r="AA5" s="14"/>
+      <c r="AB5" s="14"/>
+      <c r="AC5" s="14"/>
+      <c r="AD5" s="14"/>
+      <c r="AE5" s="14"/>
+      <c r="AF5" s="14"/>
+      <c r="AG5" s="14"/>
+      <c r="AH5" s="14"/>
+      <c r="AJ5" s="14"/>
+      <c r="AK5" s="14"/>
+    </row>
+    <row r="11" spans="1:43" x14ac:dyDescent="0.25">
       <c r="C11" s="14"/>
       <c r="D11" s="14"/>
       <c r="E11" s="14"/>
@@ -2189,7 +2124,7 @@
       <c r="J11" s="14"/>
       <c r="K11" s="14"/>
     </row>
-    <row r="12" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:43" x14ac:dyDescent="0.25">
       <c r="C12" s="14"/>
       <c r="D12" s="14"/>
       <c r="E12" s="14"/>
@@ -2200,7 +2135,7 @@
       <c r="J12" s="14"/>
       <c r="K12" s="14"/>
     </row>
-    <row r="13" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:43" x14ac:dyDescent="0.25">
       <c r="C13" s="14"/>
       <c r="D13" s="14"/>
       <c r="E13" s="14"/>
@@ -2211,7 +2146,7 @@
       <c r="J13" s="14"/>
       <c r="K13" s="14"/>
     </row>
-    <row r="14" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:43" x14ac:dyDescent="0.25">
       <c r="C14" s="14"/>
       <c r="D14" s="14"/>
       <c r="E14" s="14"/>
@@ -2222,7 +2157,7 @@
       <c r="J14" s="14"/>
       <c r="K14" s="14"/>
     </row>
-    <row r="15" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:43" x14ac:dyDescent="0.25">
       <c r="C15" s="14"/>
       <c r="D15" s="14"/>
       <c r="E15" s="14"/>
@@ -2233,7 +2168,7 @@
       <c r="J15" s="14"/>
       <c r="K15" s="14"/>
     </row>
-    <row r="16" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:43" x14ac:dyDescent="0.25">
       <c r="C16" s="14"/>
       <c r="D16" s="14"/>
       <c r="E16" s="14"/>
@@ -2244,7 +2179,7 @@
       <c r="J16" s="14"/>
       <c r="K16" s="14"/>
     </row>
-    <row r="17" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C17" s="14"/>
       <c r="D17" s="14"/>
       <c r="E17" s="14"/>
@@ -2270,30 +2205,30 @@
       <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="34" width="10.6640625" customWidth="1"/>
-    <col min="35" max="35" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="36" max="37" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="41" max="42" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="34" width="10.7109375" customWidth="1"/>
+    <col min="35" max="35" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="36" max="37" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="41" max="42" width="8.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:43" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>16</v>
       </c>
@@ -2306,7 +2241,7 @@
       <c r="AO2" s="3"/>
       <c r="AP2" s="3"/>
     </row>
-    <row r="3" spans="1:43" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="4" t="s">
         <v>9</v>
       </c>

</xml_diff>